<commit_message>
new full data position
</commit_message>
<xml_diff>
--- a/Encode_Decode/draw/data/data_position.xlsx
+++ b/Encode_Decode/draw/data/data_position.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\OOC\LEDs_Data_Processing\Encode_Decode\draw\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBBBE1A8-DDC6-4A50-A80F-6064EAD30E55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E2B20ED-5731-454F-9832-D83FCE6575D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-15" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="yaw0pitch0roll0" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,9 @@
     <sheet name="yaw0pitch20roll10" sheetId="3" r:id="rId3"/>
     <sheet name="yaw90pitch0roll0" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">yaw0pitch0roll0!$J$1:$J$226</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -504,8 +507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K226"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1087,7 +1090,7 @@
         <v>68.680000000000007</v>
       </c>
       <c r="F15" s="1">
-        <v>115.4</v>
+        <v>118.4</v>
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
@@ -1099,15 +1102,15 @@
       </c>
       <c r="I15">
         <f t="shared" si="2"/>
-        <v>-9.5999999999999943</v>
+        <v>-6.5999999999999943</v>
       </c>
       <c r="J15">
-        <f t="shared" si="4"/>
+        <f xml:space="preserve"> SQRT(G15*G15+H15*H15)</f>
         <v>10.73119285075057</v>
       </c>
       <c r="K15">
         <f t="shared" si="3"/>
-        <v>14.398558955673309</v>
+        <v>12.598353066968716</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1527,7 +1530,7 @@
         <v>24.04</v>
       </c>
       <c r="F26" s="1">
-        <v>112.29</v>
+        <v>117.29</v>
       </c>
       <c r="G26">
         <f t="shared" si="0"/>
@@ -1539,7 +1542,7 @@
       </c>
       <c r="I26">
         <f t="shared" si="2"/>
-        <v>-12.709999999999994</v>
+        <v>-7.7099999999999937</v>
       </c>
       <c r="J26">
         <f t="shared" si="4"/>
@@ -1547,7 +1550,7 @@
       </c>
       <c r="K26">
         <f t="shared" si="3"/>
-        <v>13.646164296240897</v>
+        <v>9.1715756552513863</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -2407,7 +2410,7 @@
         <v>-62.16</v>
       </c>
       <c r="F48" s="1">
-        <v>112.32</v>
+        <v>116.32</v>
       </c>
       <c r="G48">
         <f t="shared" si="0"/>
@@ -2419,7 +2422,7 @@
       </c>
       <c r="I48">
         <f t="shared" si="2"/>
-        <v>-12.680000000000007</v>
+        <v>-8.6800000000000068</v>
       </c>
       <c r="J48">
         <f t="shared" si="4"/>
@@ -2427,7 +2430,7 @@
       </c>
       <c r="K48">
         <f t="shared" si="3"/>
-        <v>13.264448725823481</v>
+        <v>9.5134431201326954</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
@@ -3524,10 +3527,10 @@
         <v>-32.96</v>
       </c>
       <c r="E76" s="1">
-        <v>81.48</v>
+        <v>78.48</v>
       </c>
       <c r="F76" s="1">
-        <v>112.29</v>
+        <v>120.29</v>
       </c>
       <c r="G76">
         <f t="shared" si="5"/>
@@ -3535,19 +3538,19 @@
       </c>
       <c r="H76">
         <f t="shared" si="6"/>
-        <v>11.480000000000004</v>
+        <v>8.480000000000004</v>
       </c>
       <c r="I76">
         <f t="shared" si="7"/>
-        <v>-12.709999999999994</v>
+        <v>-4.7099999999999937</v>
       </c>
       <c r="J76">
-        <f t="shared" si="8"/>
-        <v>11.855462875822273</v>
+        <f xml:space="preserve"> SQRT(G76*G76+H76*H76)</f>
+        <v>8.9817592931451955</v>
       </c>
       <c r="K76">
         <f t="shared" si="9"/>
-        <v>17.380911943853807</v>
+        <v>10.141799643061384</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
@@ -3887,7 +3890,7 @@
         <v>13.78</v>
       </c>
       <c r="F85" s="1">
-        <v>109.07</v>
+        <v>115.07</v>
       </c>
       <c r="G85">
         <f t="shared" si="5"/>
@@ -3899,7 +3902,7 @@
       </c>
       <c r="I85">
         <f t="shared" si="7"/>
-        <v>-15.930000000000007</v>
+        <v>-9.9300000000000068</v>
       </c>
       <c r="J85">
         <f t="shared" si="8"/>
@@ -3907,7 +3910,7 @@
       </c>
       <c r="K85">
         <f t="shared" si="9"/>
-        <v>16.593471607834214</v>
+        <v>10.962814419664328</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
@@ -6927,7 +6930,7 @@
         <v>23.03</v>
       </c>
       <c r="F161" s="1">
-        <v>112.32</v>
+        <v>116.32</v>
       </c>
       <c r="G161">
         <f t="shared" si="10"/>
@@ -6939,7 +6942,7 @@
       </c>
       <c r="I161">
         <f t="shared" si="12"/>
-        <v>-12.680000000000007</v>
+        <v>-8.6800000000000068</v>
       </c>
       <c r="J161">
         <f t="shared" si="13"/>
@@ -6947,7 +6950,7 @@
       </c>
       <c r="K161">
         <f t="shared" si="14"/>
-        <v>13.085877884192568</v>
+        <v>9.2628397373591707</v>
       </c>
     </row>
     <row r="162" spans="1:11" x14ac:dyDescent="0.25">
@@ -8607,7 +8610,7 @@
         <v>-10.39</v>
       </c>
       <c r="F203" s="1">
-        <v>112.29</v>
+        <v>116.29</v>
       </c>
       <c r="G203">
         <f t="shared" si="16"/>
@@ -8619,7 +8622,7 @@
       </c>
       <c r="I203">
         <f t="shared" si="18"/>
-        <v>-12.709999999999994</v>
+        <v>-8.7099999999999937</v>
       </c>
       <c r="J203">
         <f t="shared" si="15"/>
@@ -8627,7 +8630,7 @@
       </c>
       <c r="K203">
         <f t="shared" si="19"/>
-        <v>13.468845533303877</v>
+        <v>9.7841606691631888</v>
       </c>
     </row>
     <row r="204" spans="1:11" x14ac:dyDescent="0.25">
@@ -11441,7 +11444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>

</xml_diff>